<commit_message>
Separate function from front-end html
</commit_message>
<xml_diff>
--- a/test_file/sum_test_240410.xlsx
+++ b/test_file/sum_test_240410.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Desktop/my_github/auto-excel-changer/test_file/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{052CF07B-C773-B341-BD07-C58C74F28DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03CB14DE-6A06-1442-8B32-32AB485DB54D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="2160" windowWidth="28300" windowHeight="17440" xr2:uid="{3EDB6DFD-EF21-DF4F-A08A-70611F58BC65}"/>
   </bookViews>
@@ -406,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8AE1A35-4329-3749-92C9-861C278329A5}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -424,7 +424,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -448,10 +448,18 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5">
         <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add divide and multiply results
</commit_message>
<xml_diff>
--- a/test_file/sum_test_240410.xlsx
+++ b/test_file/sum_test_240410.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Desktop/my_github/auto-excel-changer/test_file/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03CB14DE-6A06-1442-8B32-32AB485DB54D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E3D09E-B1DF-464B-A2D0-62C31729DC57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="2160" windowWidth="28300" windowHeight="17440" xr2:uid="{3EDB6DFD-EF21-DF4F-A08A-70611F58BC65}"/>
   </bookViews>
@@ -409,7 +409,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>

</xml_diff>